<commit_message>
Updated. Test is now running in Chrome.
</commit_message>
<xml_diff>
--- a/karma-ts-howto.xlsx
+++ b/karma-ts-howto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Ivy\Github\karma-typescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE981B6-09C0-4BA1-93AB-40714A75D8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38FEDCB-A9CF-48F3-AA9D-C5DDE3BD1B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="771" activeTab="3" xr2:uid="{F8FD7D67-54D6-4F97-86DC-2E3CAB04B120}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="771" activeTab="2" xr2:uid="{F8FD7D67-54D6-4F97-86DC-2E3CAB04B120}"/>
   </bookViews>
   <sheets>
     <sheet name="Installation and Configuration" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
   <si>
     <t>Prerequisite:</t>
   </si>
@@ -288,40 +288,6 @@
     <t>File Heirarchy</t>
   </si>
   <si>
-    <t>{
-  "name": "sample-karma-test",
-  "version": "1.0.0",
-  "description": "Karma test sample",
-  "scripts": {
-    "test": "karma start karma.conf.js"
-  },
-  "author": "Your Name",
-  "devDependencies": {
-    "chai": "^2.1.0",
-    "core-util-is": "^1.0.2",
-    "gulp": "^4.0.2",
-    "istanbul": "^0.3.6",
-    "jshint": "^2.6.0",
-    "karma": "^0.12.37",
-    "karma-chai": "^0.1.0",
-    "karma-chrome-launcher": "^0.1.7",
-    "karma-cli": "0.0.4",
-    "karma-coverage": "^0.2.7",
-    "karma-fixture": "^0.2.1-1",
-    "karma-html-reporter": "^0.2.7",
-    "karma-html2js-preprocessor": "*",
-    "karma-htmlfile-reporter": "^0.3.8",
-    "karma-ie-launcher": "^1.0.0",
-    "karma-jasmine-html-reporter": "^1.5.3",
-    "karma-mocha": "^0.1.10",
-    "karma-ng-html2js-preprocessor": "^1.0.0",
-    "karma-phantomjs-launcher": "^0.1.4",
-    "mocha": "^2.1.0",
-    "webpack-dev-server": "^3.10.3"
-  }
-}</t>
-  </si>
-  <si>
     <t>Summary of execution is added to 'test' folder as specified on karma.conf.js file's htmlReporter.outputFile.</t>
   </si>
   <si>
@@ -350,25 +316,6 @@
     <t>Accessing file</t>
   </si>
   <si>
-    <t>function isMatching(str1, str2) {
-    if (str1 === str2) {
-        return true;
-    } else {
-        return false;
-    }
-};</t>
-  </si>
-  <si>
-    <t>describe('#isMatching()', function() {
-   it('returns true if the values match', function() {
-      assert.equal(true, isMatching("hello", "hello"));
-   });
-   it('returns false if the values does not match', function() {
-      assert.equal(false, isMatching("hello", "hi"));
-   });
-});</t>
-  </si>
-  <si>
     <t>Without accessing file</t>
   </si>
   <si>
@@ -379,162 +326,6 @@
   </si>
   <si>
     <t>Sample output during execution:</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">module.exports = function (config) {
-    config.set({
-      frameworks: ['mocha', 'chai'],
-      files: [ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>//files to be used for execution</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-          './src/*.js',
-          './test/*.js'
-      ],
-      preprocessors: { //</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>source files to generate coverage report</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-          './src/*.js': 'coverage'
-      },
-      reporters: ['progress', 'coverage', 'html'],
-      htmlReporter: {
-          outputFile: './test/test-results.html' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>//test result output</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-      },
-      port: 9876,  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>// karma web server port</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-      colors: true,
-      client: {
-          clearContext: false
-      },
-      logLevel: config.LOG_INFO,
-      browsers: ['Chrome', 'IE'],</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> //browsers to be used for execution</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-      autoWatch: false,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> //enable/disable watching files</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-      concurrency: Infinity,
-      singleRun: true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> //if true, start and capture all configured browsers then run tests</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-  })
-}</t>
-    </r>
   </si>
   <si>
     <t>Typescript is not included on installation so you should manually install Typescript.</t>
@@ -937,12 +728,146 @@
   <si>
     <t>npm install --save-dev @types/mocha</t>
   </si>
+  <si>
+    <t>When browser (in this case, I used Chrome) is launched, click "DEBUG".</t>
+  </si>
+  <si>
+    <t>It will open a blank page on new tab. Open Chrome Developer Tools and on Console, check what causes the error.</t>
+  </si>
+  <si>
+    <t>7. Tests are not executed when using Chrome (Executed 0 of 0 ERROR)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set mime property to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>karma.conf.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>module.exports = function (config) {
+    config.set({
+      ...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+      mime: {
+        "text/x-typescript": ["ts", "tsx"]
+      },
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">      ...
+    })
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>function addNumber(a: number, b: number) : number {
+  return a + b;
+};</t>
+  </si>
+  <si>
+    <t>describe('#addNumber()', function() {
+   it('will add', function() {
+      expect(addNumber(10, 5).toBe(15);
+   });
+});</t>
+  </si>
+  <si>
+    <t>{
+  "name": "sample-karma-ts-test",
+  "version": "1.0.0",
+  "description": "Karma test sample",
+  "scripts": {
+    "test": "karma start karma.conf.js"
+  },
+  "author": "Ivy",
+  "devDependencies": {
+    "@types/jasmine": "^3.4.0",
+    "jasmine-core": "^3.4.0",
+    "karma": "^4.3.0",
+    "karma-chrome-launcher": "^3.1.0",
+    "karma-cli": "^2.0.0",
+    "karma-htmlfile-reporter": "^0.3.8",
+    "karma-ie-launcher": "^1.0.0",
+    "karma-jasmine": "^2.0.1",
+    "karma-typescript": "latest",
+    "typescript": "1.6.2"
+  }
+}</t>
+  </si>
+  <si>
+    <t>module.exports = function(config) {
+    config.set({
+        frameworks: ["jasmine", "karma-typescript"],
+        files: [
+            { pattern: "src/*.ts" },
+            { pattern: "test/*.ts"}
+        ],
+        preprocessors: {
+            "./src/*.ts": ["karma-typescript"]
+        },
+        reporters: ["progress", "html", "karma-typescript"],
+        htmlReporter: {
+            outputFile: "./test/test-results.html"
+        },
+        mime: {
+            "text/x-typescript": ["ts", "tsx"]
+        },
+        port: 9876,  // karma web server port
+        colors: true,
+        client: {
+            clearContext: false
+        },
+        logLevel: config.LOG_INFO,
+        browsers: ["Chrome", "IE"],
+        autoWatch: false,
+        concurrency: Infinity,
+        singleRun: true
+    });
+};</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1032,6 +957,24 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1047,7 +990,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1150,11 +1093,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1264,6 +1244,50 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1279,6 +1303,254 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>541957</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>171214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFEDCBDD-A054-4633-9DEC-ABCF0CDE46DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="8134350"/>
+          <a:ext cx="7742857" cy="1885714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A223FB93-8EB8-4B18-8D77-D7F5A4FEDF7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="9791700"/>
+          <a:ext cx="5581650" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>427976</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>171381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DE64949-C960-4574-8081-12CA2A9FDCA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="10610850"/>
+          <a:ext cx="5190476" cy="552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Speech Bubble: Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80D8806D-00C1-4371-9631-A4AD9C00CECC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7124699" y="10506075"/>
+          <a:ext cx="3076575" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -99014"/>
+            <a:gd name="adj2" fmla="val -1050"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>Tested both IE and Chrome.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>Chrome:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
+            <a:t> MIME type error</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
+            <a:t>IE: OK</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1846,7 +2118,7 @@
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
@@ -1859,7 +2131,7 @@
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D33" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
@@ -1883,7 +2155,7 @@
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1896,7 +2168,7 @@
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D36" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -1909,7 +2181,7 @@
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1932,7 +2204,7 @@
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
@@ -1945,12 +2217,12 @@
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
@@ -1986,12 +2258,12 @@
     </row>
     <row r="48" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D49" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
@@ -2004,12 +2276,12 @@
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D52" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
@@ -2065,12 +2337,12 @@
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D65" s="14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
@@ -2204,12 +2476,12 @@
     </row>
     <row r="78" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D79" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
@@ -2222,17 +2494,17 @@
     </row>
     <row r="80" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
@@ -2255,12 +2527,12 @@
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
@@ -2291,7 +2563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC732316-EC1A-4386-A955-03D9EA5A8CC0}">
   <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B12" sqref="B12:J23"/>
     </sheetView>
   </sheetViews>
@@ -2302,22 +2574,22 @@
   <sheetData>
     <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -2340,12 +2612,12 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -2488,10 +2760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6C7849-FFE0-44AA-A86A-9E4A7026ED91}">
-  <dimension ref="B3:X112"/>
+  <dimension ref="B3:Y98"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2535,7 +2807,7 @@
     <row r="9" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -2567,10 +2839,10 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2578,12 +2850,12 @@
         <v>24</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
@@ -2594,7 +2866,7 @@
       <c r="J17" s="24"/>
       <c r="K17" s="25"/>
       <c r="Q17" s="23" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="R17" s="33"/>
       <c r="S17" s="33"/>
@@ -2604,7 +2876,7 @@
       <c r="W17" s="33"/>
       <c r="X17" s="34"/>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C18" s="26"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
@@ -2623,7 +2895,7 @@
       <c r="W18" s="36"/>
       <c r="X18" s="37"/>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C19" s="26"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
@@ -2642,7 +2914,7 @@
       <c r="W19" s="36"/>
       <c r="X19" s="37"/>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C20" s="26"/>
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
@@ -2652,16 +2924,16 @@
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
       <c r="K20" s="28"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="37"/>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Q20" s="38"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="39"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="39"/>
+      <c r="X20" s="40"/>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C21" s="29"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
@@ -2671,48 +2943,57 @@
       <c r="I21" s="30"/>
       <c r="J21" s="30"/>
       <c r="K21" s="31"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="37"/>
-    </row>
-    <row r="22" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Q21" s="54"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="55"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
+      <c r="X21" s="55"/>
+      <c r="Y21" s="56"/>
+    </row>
+    <row r="22" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="39"/>
-      <c r="S22" s="39"/>
-      <c r="T22" s="39"/>
-      <c r="U22" s="39"/>
-      <c r="V22" s="39"/>
-      <c r="W22" s="39"/>
-      <c r="X22" s="40"/>
-    </row>
-    <row r="23" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M22" s="56"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="56"/>
+      <c r="S22" s="56"/>
+      <c r="T22" s="56"/>
+      <c r="U22" s="56"/>
+      <c r="V22" s="56"/>
+      <c r="W22" s="56"/>
+      <c r="X22" s="56"/>
+    </row>
+    <row r="23" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="P24" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="Q25" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="33"/>
-      <c r="W25" s="33"/>
-      <c r="X25" s="34"/>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Q24" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="34"/>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Q25" s="35"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="36"/>
+      <c r="V25" s="36"/>
+      <c r="W25" s="36"/>
+      <c r="X25" s="37"/>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q26" s="35"/>
       <c r="R26" s="36"/>
       <c r="S26" s="36"/>
@@ -2722,7 +3003,7 @@
       <c r="W26" s="36"/>
       <c r="X26" s="37"/>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q27" s="35"/>
       <c r="R27" s="36"/>
       <c r="S27" s="36"/>
@@ -2732,117 +3013,121 @@
       <c r="W27" s="36"/>
       <c r="X27" s="37"/>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="Q28" s="35"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="36"/>
-      <c r="W28" s="36"/>
-      <c r="X28" s="37"/>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="Q29" s="35"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="T29" s="36"/>
-      <c r="U29" s="36"/>
-      <c r="V29" s="36"/>
-      <c r="W29" s="36"/>
-      <c r="X29" s="37"/>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="Q30" s="35"/>
-      <c r="R30" s="36"/>
-      <c r="S30" s="36"/>
-      <c r="T30" s="36"/>
-      <c r="U30" s="36"/>
-      <c r="V30" s="36"/>
-      <c r="W30" s="36"/>
-      <c r="X30" s="37"/>
-    </row>
-    <row r="31" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36"/>
-      <c r="U31" s="36"/>
-      <c r="V31" s="36"/>
-      <c r="W31" s="36"/>
-      <c r="X31" s="37"/>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="Q32" s="35"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="36"/>
-      <c r="U32" s="36"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="37"/>
-    </row>
-    <row r="33" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="36"/>
-      <c r="S33" s="36"/>
-      <c r="T33" s="36"/>
-      <c r="U33" s="36"/>
-      <c r="V33" s="36"/>
-      <c r="W33" s="36"/>
-      <c r="X33" s="37"/>
-    </row>
-    <row r="34" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B34" s="2"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="36"/>
-      <c r="S34" s="36"/>
-      <c r="T34" s="36"/>
-      <c r="U34" s="36"/>
-      <c r="V34" s="36"/>
-      <c r="W34" s="36"/>
-      <c r="X34" s="37"/>
-    </row>
-    <row r="35" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B35" s="2"/>
-      <c r="Q35" s="38"/>
-      <c r="R35" s="39"/>
-      <c r="S35" s="39"/>
-      <c r="T35" s="39"/>
-      <c r="U35" s="39"/>
-      <c r="V35" s="39"/>
-      <c r="W35" s="39"/>
-      <c r="X35" s="40"/>
-    </row>
-    <row r="36" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="38" spans="2:24" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B38" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+    <row r="28" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
+      <c r="T28" s="39"/>
+      <c r="U28" s="39"/>
+      <c r="V28" s="39"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="40"/>
+    </row>
+    <row r="29" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="31" spans="2:25" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C41" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="25"/>
-    </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="25"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C35" s="26"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="28"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="26"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="28"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C37" s="26"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="28"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C38" s="26"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="28"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C39" s="26"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="28"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C40" s="26"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="28"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C41" s="26"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="28"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C42" s="26"/>
       <c r="D42" s="32"/>
       <c r="E42" s="32"/>
@@ -2853,7 +3138,7 @@
       <c r="J42" s="32"/>
       <c r="K42" s="28"/>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C43" s="26"/>
       <c r="D43" s="32"/>
       <c r="E43" s="32"/>
@@ -2864,7 +3149,7 @@
       <c r="J43" s="32"/>
       <c r="K43" s="28"/>
     </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C44" s="26"/>
       <c r="D44" s="32"/>
       <c r="E44" s="32"/>
@@ -2875,7 +3160,7 @@
       <c r="J44" s="32"/>
       <c r="K44" s="28"/>
     </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C45" s="26"/>
       <c r="D45" s="32"/>
       <c r="E45" s="32"/>
@@ -2886,7 +3171,7 @@
       <c r="J45" s="32"/>
       <c r="K45" s="28"/>
     </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C46" s="26"/>
       <c r="D46" s="32"/>
       <c r="E46" s="32"/>
@@ -2897,7 +3182,7 @@
       <c r="J46" s="32"/>
       <c r="K46" s="28"/>
     </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C47" s="26"/>
       <c r="D47" s="32"/>
       <c r="E47" s="32"/>
@@ -2908,7 +3193,7 @@
       <c r="J47" s="32"/>
       <c r="K47" s="28"/>
     </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C48" s="26"/>
       <c r="D48" s="32"/>
       <c r="E48" s="32"/>
@@ -2919,7 +3204,7 @@
       <c r="J48" s="32"/>
       <c r="K48" s="28"/>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C49" s="26"/>
       <c r="D49" s="32"/>
       <c r="E49" s="32"/>
@@ -2930,7 +3215,7 @@
       <c r="J49" s="32"/>
       <c r="K49" s="28"/>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C50" s="26"/>
       <c r="D50" s="32"/>
       <c r="E50" s="32"/>
@@ -2941,7 +3226,7 @@
       <c r="J50" s="32"/>
       <c r="K50" s="28"/>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C51" s="26"/>
       <c r="D51" s="32"/>
       <c r="E51" s="32"/>
@@ -2952,62 +3237,56 @@
       <c r="J51" s="32"/>
       <c r="K51" s="28"/>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C52" s="26"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="28"/>
-    </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C53" s="26"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="28"/>
-    </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C54" s="26"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="28"/>
-    </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C55" s="26"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="28"/>
-    </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C56" s="26"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="28"/>
-    </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C52" s="29"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="30"/>
+      <c r="K52" s="31"/>
+    </row>
+    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+    </row>
+    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C56" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="25"/>
+      <c r="N56" s="55"/>
+      <c r="O56" s="55"/>
+      <c r="P56" s="55"/>
+      <c r="Q56" s="55"/>
+      <c r="R56" s="55"/>
+      <c r="S56" s="55"/>
+      <c r="T56" s="55"/>
+      <c r="U56" s="55"/>
+      <c r="V56" s="55"/>
+    </row>
+    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C57" s="26"/>
       <c r="D57" s="32"/>
       <c r="E57" s="32"/>
@@ -3017,8 +3296,17 @@
       <c r="I57" s="32"/>
       <c r="J57" s="32"/>
       <c r="K57" s="28"/>
-    </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N57" s="55"/>
+      <c r="O57" s="55"/>
+      <c r="P57" s="55"/>
+      <c r="Q57" s="55"/>
+      <c r="R57" s="55"/>
+      <c r="S57" s="55"/>
+      <c r="T57" s="55"/>
+      <c r="U57" s="55"/>
+      <c r="V57" s="55"/>
+    </row>
+    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C58" s="26"/>
       <c r="D58" s="32"/>
       <c r="E58" s="32"/>
@@ -3028,8 +3316,17 @@
       <c r="I58" s="32"/>
       <c r="J58" s="32"/>
       <c r="K58" s="28"/>
-    </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N58" s="55"/>
+      <c r="O58" s="55"/>
+      <c r="P58" s="55"/>
+      <c r="Q58" s="55"/>
+      <c r="R58" s="55"/>
+      <c r="S58" s="55"/>
+      <c r="T58" s="55"/>
+      <c r="U58" s="55"/>
+      <c r="V58" s="55"/>
+    </row>
+    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C59" s="26"/>
       <c r="D59" s="32"/>
       <c r="E59" s="32"/>
@@ -3039,8 +3336,17 @@
       <c r="I59" s="32"/>
       <c r="J59" s="32"/>
       <c r="K59" s="28"/>
-    </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N59" s="55"/>
+      <c r="O59" s="55"/>
+      <c r="P59" s="55"/>
+      <c r="Q59" s="55"/>
+      <c r="R59" s="55"/>
+      <c r="S59" s="55"/>
+      <c r="T59" s="55"/>
+      <c r="U59" s="55"/>
+      <c r="V59" s="55"/>
+    </row>
+    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C60" s="26"/>
       <c r="D60" s="32"/>
       <c r="E60" s="32"/>
@@ -3050,8 +3356,17 @@
       <c r="I60" s="32"/>
       <c r="J60" s="32"/>
       <c r="K60" s="28"/>
-    </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N60" s="55"/>
+      <c r="O60" s="55"/>
+      <c r="P60" s="55"/>
+      <c r="Q60" s="55"/>
+      <c r="R60" s="55"/>
+      <c r="S60" s="55"/>
+      <c r="T60" s="55"/>
+      <c r="U60" s="55"/>
+      <c r="V60" s="55"/>
+    </row>
+    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C61" s="26"/>
       <c r="D61" s="32"/>
       <c r="E61" s="32"/>
@@ -3061,8 +3376,17 @@
       <c r="I61" s="32"/>
       <c r="J61" s="32"/>
       <c r="K61" s="28"/>
-    </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N61" s="55"/>
+      <c r="O61" s="55"/>
+      <c r="P61" s="55"/>
+      <c r="Q61" s="55"/>
+      <c r="R61" s="55"/>
+      <c r="S61" s="55"/>
+      <c r="T61" s="55"/>
+      <c r="U61" s="55"/>
+      <c r="V61" s="55"/>
+    </row>
+    <row r="62" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C62" s="26"/>
       <c r="D62" s="32"/>
       <c r="E62" s="32"/>
@@ -3072,8 +3396,17 @@
       <c r="I62" s="32"/>
       <c r="J62" s="32"/>
       <c r="K62" s="28"/>
-    </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N62" s="55"/>
+      <c r="O62" s="55"/>
+      <c r="P62" s="55"/>
+      <c r="Q62" s="55"/>
+      <c r="R62" s="55"/>
+      <c r="S62" s="55"/>
+      <c r="T62" s="55"/>
+      <c r="U62" s="55"/>
+      <c r="V62" s="55"/>
+    </row>
+    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C63" s="26"/>
       <c r="D63" s="32"/>
       <c r="E63" s="32"/>
@@ -3083,8 +3416,17 @@
       <c r="I63" s="32"/>
       <c r="J63" s="32"/>
       <c r="K63" s="28"/>
-    </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N63" s="55"/>
+      <c r="O63" s="55"/>
+      <c r="P63" s="55"/>
+      <c r="Q63" s="55"/>
+      <c r="R63" s="55"/>
+      <c r="S63" s="55"/>
+      <c r="T63" s="55"/>
+      <c r="U63" s="55"/>
+      <c r="V63" s="55"/>
+    </row>
+    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C64" s="26"/>
       <c r="D64" s="32"/>
       <c r="E64" s="32"/>
@@ -3094,8 +3436,17 @@
       <c r="I64" s="32"/>
       <c r="J64" s="32"/>
       <c r="K64" s="28"/>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N64" s="55"/>
+      <c r="O64" s="55"/>
+      <c r="P64" s="55"/>
+      <c r="Q64" s="55"/>
+      <c r="R64" s="55"/>
+      <c r="S64" s="55"/>
+      <c r="T64" s="55"/>
+      <c r="U64" s="55"/>
+      <c r="V64" s="55"/>
+    </row>
+    <row r="65" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C65" s="26"/>
       <c r="D65" s="32"/>
       <c r="E65" s="32"/>
@@ -3105,8 +3456,17 @@
       <c r="I65" s="32"/>
       <c r="J65" s="32"/>
       <c r="K65" s="28"/>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N65" s="55"/>
+      <c r="O65" s="55"/>
+      <c r="P65" s="55"/>
+      <c r="Q65" s="55"/>
+      <c r="R65" s="55"/>
+      <c r="S65" s="55"/>
+      <c r="T65" s="55"/>
+      <c r="U65" s="55"/>
+      <c r="V65" s="55"/>
+    </row>
+    <row r="66" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C66" s="26"/>
       <c r="D66" s="32"/>
       <c r="E66" s="32"/>
@@ -3116,8 +3476,17 @@
       <c r="I66" s="32"/>
       <c r="J66" s="32"/>
       <c r="K66" s="28"/>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N66" s="55"/>
+      <c r="O66" s="55"/>
+      <c r="P66" s="55"/>
+      <c r="Q66" s="55"/>
+      <c r="R66" s="55"/>
+      <c r="S66" s="55"/>
+      <c r="T66" s="55"/>
+      <c r="U66" s="55"/>
+      <c r="V66" s="55"/>
+    </row>
+    <row r="67" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C67" s="26"/>
       <c r="D67" s="32"/>
       <c r="E67" s="32"/>
@@ -3127,48 +3496,117 @@
       <c r="I67" s="32"/>
       <c r="J67" s="32"/>
       <c r="K67" s="28"/>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C68" s="29"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
-      <c r="J68" s="30"/>
-      <c r="K68" s="31"/>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C72" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="24"/>
-      <c r="I72" s="24"/>
-      <c r="J72" s="24"/>
-      <c r="K72" s="25"/>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N67" s="55"/>
+      <c r="O67" s="55"/>
+      <c r="P67" s="55"/>
+      <c r="Q67" s="55"/>
+      <c r="R67" s="55"/>
+      <c r="S67" s="55"/>
+      <c r="T67" s="55"/>
+      <c r="U67" s="55"/>
+      <c r="V67" s="55"/>
+    </row>
+    <row r="68" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C68" s="26"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
+      <c r="I68" s="32"/>
+      <c r="J68" s="32"/>
+      <c r="K68" s="28"/>
+      <c r="N68" s="55"/>
+      <c r="O68" s="55"/>
+      <c r="P68" s="55"/>
+      <c r="Q68" s="55"/>
+      <c r="R68" s="55"/>
+      <c r="S68" s="55"/>
+      <c r="T68" s="55"/>
+      <c r="U68" s="55"/>
+      <c r="V68" s="55"/>
+    </row>
+    <row r="69" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C69" s="26"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="32"/>
+      <c r="J69" s="32"/>
+      <c r="K69" s="28"/>
+      <c r="N69" s="55"/>
+      <c r="O69" s="55"/>
+      <c r="P69" s="55"/>
+      <c r="Q69" s="55"/>
+      <c r="R69" s="55"/>
+      <c r="S69" s="55"/>
+      <c r="T69" s="55"/>
+      <c r="U69" s="55"/>
+      <c r="V69" s="55"/>
+    </row>
+    <row r="70" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C70" s="26"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="32"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="32"/>
+      <c r="J70" s="32"/>
+      <c r="K70" s="28"/>
+      <c r="N70" s="55"/>
+      <c r="O70" s="55"/>
+      <c r="P70" s="55"/>
+      <c r="Q70" s="55"/>
+      <c r="R70" s="55"/>
+      <c r="S70" s="55"/>
+      <c r="T70" s="55"/>
+      <c r="U70" s="55"/>
+      <c r="V70" s="55"/>
+    </row>
+    <row r="71" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C71" s="26"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="32"/>
+      <c r="K71" s="28"/>
+      <c r="N71" s="55"/>
+      <c r="O71" s="55"/>
+      <c r="P71" s="55"/>
+      <c r="Q71" s="55"/>
+      <c r="R71" s="55"/>
+      <c r="S71" s="55"/>
+      <c r="T71" s="55"/>
+      <c r="U71" s="55"/>
+      <c r="V71" s="55"/>
+    </row>
+    <row r="72" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C72" s="26"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="32"/>
+      <c r="K72" s="28"/>
+      <c r="N72" s="55"/>
+      <c r="O72" s="55"/>
+      <c r="P72" s="55"/>
+      <c r="Q72" s="55"/>
+      <c r="R72" s="55"/>
+      <c r="S72" s="55"/>
+      <c r="T72" s="55"/>
+      <c r="U72" s="55"/>
+      <c r="V72" s="55"/>
+    </row>
+    <row r="73" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C73" s="26"/>
       <c r="D73" s="32"/>
       <c r="E73" s="32"/>
@@ -3178,8 +3616,17 @@
       <c r="I73" s="32"/>
       <c r="J73" s="32"/>
       <c r="K73" s="28"/>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N73" s="55"/>
+      <c r="O73" s="55"/>
+      <c r="P73" s="55"/>
+      <c r="Q73" s="55"/>
+      <c r="R73" s="55"/>
+      <c r="S73" s="55"/>
+      <c r="T73" s="55"/>
+      <c r="U73" s="55"/>
+      <c r="V73" s="55"/>
+    </row>
+    <row r="74" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C74" s="26"/>
       <c r="D74" s="32"/>
       <c r="E74" s="32"/>
@@ -3189,8 +3636,17 @@
       <c r="I74" s="32"/>
       <c r="J74" s="32"/>
       <c r="K74" s="28"/>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N74" s="55"/>
+      <c r="O74" s="55"/>
+      <c r="P74" s="55"/>
+      <c r="Q74" s="55"/>
+      <c r="R74" s="55"/>
+      <c r="S74" s="55"/>
+      <c r="T74" s="55"/>
+      <c r="U74" s="55"/>
+      <c r="V74" s="55"/>
+    </row>
+    <row r="75" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C75" s="26"/>
       <c r="D75" s="32"/>
       <c r="E75" s="32"/>
@@ -3200,8 +3656,17 @@
       <c r="I75" s="32"/>
       <c r="J75" s="32"/>
       <c r="K75" s="28"/>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N75" s="55"/>
+      <c r="O75" s="55"/>
+      <c r="P75" s="55"/>
+      <c r="Q75" s="55"/>
+      <c r="R75" s="55"/>
+      <c r="S75" s="55"/>
+      <c r="T75" s="55"/>
+      <c r="U75" s="55"/>
+      <c r="V75" s="55"/>
+    </row>
+    <row r="76" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C76" s="26"/>
       <c r="D76" s="32"/>
       <c r="E76" s="32"/>
@@ -3211,8 +3676,17 @@
       <c r="I76" s="32"/>
       <c r="J76" s="32"/>
       <c r="K76" s="28"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N76" s="55"/>
+      <c r="O76" s="55"/>
+      <c r="P76" s="55"/>
+      <c r="Q76" s="55"/>
+      <c r="R76" s="55"/>
+      <c r="S76" s="55"/>
+      <c r="T76" s="55"/>
+      <c r="U76" s="55"/>
+      <c r="V76" s="55"/>
+    </row>
+    <row r="77" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C77" s="26"/>
       <c r="D77" s="32"/>
       <c r="E77" s="32"/>
@@ -3222,8 +3696,17 @@
       <c r="I77" s="32"/>
       <c r="J77" s="32"/>
       <c r="K77" s="28"/>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N77" s="55"/>
+      <c r="O77" s="55"/>
+      <c r="P77" s="55"/>
+      <c r="Q77" s="55"/>
+      <c r="R77" s="55"/>
+      <c r="S77" s="55"/>
+      <c r="T77" s="55"/>
+      <c r="U77" s="55"/>
+      <c r="V77" s="55"/>
+    </row>
+    <row r="78" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C78" s="26"/>
       <c r="D78" s="32"/>
       <c r="E78" s="32"/>
@@ -3233,8 +3716,17 @@
       <c r="I78" s="32"/>
       <c r="J78" s="32"/>
       <c r="K78" s="28"/>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N78" s="55"/>
+      <c r="O78" s="55"/>
+      <c r="P78" s="55"/>
+      <c r="Q78" s="55"/>
+      <c r="R78" s="55"/>
+      <c r="S78" s="55"/>
+      <c r="T78" s="55"/>
+      <c r="U78" s="55"/>
+      <c r="V78" s="55"/>
+    </row>
+    <row r="79" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C79" s="26"/>
       <c r="D79" s="32"/>
       <c r="E79" s="32"/>
@@ -3244,8 +3736,17 @@
       <c r="I79" s="32"/>
       <c r="J79" s="32"/>
       <c r="K79" s="28"/>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N79" s="55"/>
+      <c r="O79" s="55"/>
+      <c r="P79" s="55"/>
+      <c r="Q79" s="55"/>
+      <c r="R79" s="55"/>
+      <c r="S79" s="55"/>
+      <c r="T79" s="55"/>
+      <c r="U79" s="55"/>
+      <c r="V79" s="55"/>
+    </row>
+    <row r="80" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C80" s="26"/>
       <c r="D80" s="32"/>
       <c r="E80" s="32"/>
@@ -3255,351 +3756,215 @@
       <c r="I80" s="32"/>
       <c r="J80" s="32"/>
       <c r="K80" s="28"/>
-    </row>
-    <row r="81" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C81" s="26"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="32"/>
-      <c r="H81" s="32"/>
-      <c r="I81" s="32"/>
-      <c r="J81" s="32"/>
-      <c r="K81" s="28"/>
-    </row>
-    <row r="82" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C82" s="26"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="32"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="32"/>
-      <c r="H82" s="32"/>
-      <c r="I82" s="32"/>
-      <c r="J82" s="32"/>
-      <c r="K82" s="28"/>
-    </row>
-    <row r="83" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C83" s="26"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="32"/>
-      <c r="F83" s="32"/>
-      <c r="G83" s="32"/>
-      <c r="H83" s="32"/>
-      <c r="I83" s="32"/>
-      <c r="J83" s="32"/>
-      <c r="K83" s="28"/>
-    </row>
-    <row r="84" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C84" s="26"/>
-      <c r="D84" s="32"/>
-      <c r="E84" s="32"/>
-      <c r="F84" s="32"/>
-      <c r="G84" s="32"/>
-      <c r="H84" s="32"/>
-      <c r="I84" s="32"/>
-      <c r="J84" s="32"/>
-      <c r="K84" s="28"/>
-    </row>
-    <row r="85" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C85" s="26"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="32"/>
-      <c r="H85" s="32"/>
-      <c r="I85" s="32"/>
-      <c r="J85" s="32"/>
-      <c r="K85" s="28"/>
-    </row>
-    <row r="86" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C86" s="26"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="32"/>
-      <c r="H86" s="32"/>
-      <c r="I86" s="32"/>
-      <c r="J86" s="32"/>
-      <c r="K86" s="28"/>
-    </row>
-    <row r="87" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C87" s="26"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="32"/>
-      <c r="G87" s="32"/>
-      <c r="H87" s="32"/>
-      <c r="I87" s="32"/>
-      <c r="J87" s="32"/>
-      <c r="K87" s="28"/>
-    </row>
-    <row r="88" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C88" s="26"/>
-      <c r="D88" s="32"/>
-      <c r="E88" s="32"/>
-      <c r="F88" s="32"/>
-      <c r="G88" s="32"/>
-      <c r="H88" s="32"/>
-      <c r="I88" s="32"/>
-      <c r="J88" s="32"/>
-      <c r="K88" s="28"/>
-    </row>
-    <row r="89" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C89" s="26"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="32"/>
-      <c r="F89" s="32"/>
-      <c r="G89" s="32"/>
-      <c r="H89" s="32"/>
-      <c r="I89" s="32"/>
-      <c r="J89" s="32"/>
-      <c r="K89" s="28"/>
-    </row>
-    <row r="90" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C90" s="26"/>
-      <c r="D90" s="32"/>
-      <c r="E90" s="32"/>
-      <c r="F90" s="32"/>
-      <c r="G90" s="32"/>
-      <c r="H90" s="32"/>
-      <c r="I90" s="32"/>
-      <c r="J90" s="32"/>
-      <c r="K90" s="28"/>
-    </row>
-    <row r="91" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C91" s="26"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="32"/>
-      <c r="F91" s="32"/>
-      <c r="G91" s="32"/>
-      <c r="H91" s="32"/>
-      <c r="I91" s="32"/>
-      <c r="J91" s="32"/>
-      <c r="K91" s="28"/>
-    </row>
-    <row r="92" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C92" s="26"/>
-      <c r="D92" s="32"/>
-      <c r="E92" s="32"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="32"/>
-      <c r="H92" s="32"/>
-      <c r="I92" s="32"/>
-      <c r="J92" s="32"/>
-      <c r="K92" s="28"/>
-    </row>
-    <row r="93" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C93" s="26"/>
-      <c r="D93" s="32"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="32"/>
-      <c r="H93" s="32"/>
-      <c r="I93" s="32"/>
-      <c r="J93" s="32"/>
-      <c r="K93" s="28"/>
-    </row>
-    <row r="94" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C94" s="26"/>
-      <c r="D94" s="32"/>
-      <c r="E94" s="32"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="32"/>
-      <c r="H94" s="32"/>
-      <c r="I94" s="32"/>
-      <c r="J94" s="32"/>
-      <c r="K94" s="28"/>
-    </row>
-    <row r="95" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C95" s="29"/>
-      <c r="D95" s="30"/>
-      <c r="E95" s="30"/>
-      <c r="F95" s="30"/>
-      <c r="G95" s="30"/>
-      <c r="H95" s="30"/>
-      <c r="I95" s="30"/>
-      <c r="J95" s="30"/>
-      <c r="K95" s="31"/>
-    </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="99" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C99" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D99" s="33"/>
-      <c r="E99" s="33"/>
-      <c r="F99" s="33"/>
-      <c r="G99" s="33"/>
-      <c r="H99" s="33"/>
-      <c r="I99" s="33"/>
-      <c r="J99" s="33"/>
-      <c r="K99" s="33"/>
-      <c r="L99" s="33"/>
-      <c r="M99" s="33"/>
-      <c r="N99" s="34"/>
-    </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C100" s="35"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="36"/>
-      <c r="F100" s="36"/>
-      <c r="G100" s="36"/>
-      <c r="H100" s="36"/>
-      <c r="I100" s="36"/>
-      <c r="J100" s="36"/>
-      <c r="K100" s="36"/>
-      <c r="L100" s="36"/>
-      <c r="M100" s="36"/>
-      <c r="N100" s="37"/>
-    </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C101" s="35"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="36"/>
-      <c r="I101" s="36"/>
-      <c r="J101" s="36"/>
-      <c r="K101" s="36"/>
-      <c r="L101" s="36"/>
-      <c r="M101" s="36"/>
-      <c r="N101" s="37"/>
-    </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C102" s="35"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="36"/>
-      <c r="F102" s="36"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="36"/>
-      <c r="I102" s="36"/>
-      <c r="J102" s="36"/>
-      <c r="K102" s="36"/>
-      <c r="L102" s="36"/>
-      <c r="M102" s="36"/>
-      <c r="N102" s="37"/>
-    </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C103" s="35"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
-      <c r="F103" s="36"/>
-      <c r="G103" s="36"/>
-      <c r="H103" s="36"/>
-      <c r="I103" s="36"/>
-      <c r="J103" s="36"/>
-      <c r="K103" s="36"/>
-      <c r="L103" s="36"/>
-      <c r="M103" s="36"/>
-      <c r="N103" s="37"/>
-    </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C104" s="35"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
-      <c r="F104" s="36"/>
-      <c r="G104" s="36"/>
-      <c r="H104" s="36"/>
-      <c r="I104" s="36"/>
-      <c r="J104" s="36"/>
-      <c r="K104" s="36"/>
-      <c r="L104" s="36"/>
-      <c r="M104" s="36"/>
-      <c r="N104" s="37"/>
-    </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C105" s="35"/>
-      <c r="D105" s="36"/>
-      <c r="E105" s="36"/>
-      <c r="F105" s="36"/>
-      <c r="G105" s="36"/>
-      <c r="H105" s="36"/>
-      <c r="I105" s="36"/>
-      <c r="J105" s="36"/>
-      <c r="K105" s="36"/>
-      <c r="L105" s="36"/>
-      <c r="M105" s="36"/>
-      <c r="N105" s="37"/>
-    </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C106" s="35"/>
-      <c r="D106" s="36"/>
-      <c r="E106" s="36"/>
-      <c r="F106" s="36"/>
-      <c r="G106" s="36"/>
-      <c r="H106" s="36"/>
-      <c r="I106" s="36"/>
-      <c r="J106" s="36"/>
-      <c r="K106" s="36"/>
-      <c r="L106" s="36"/>
-      <c r="M106" s="36"/>
-      <c r="N106" s="37"/>
-    </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C107" s="35"/>
-      <c r="D107" s="36"/>
-      <c r="E107" s="36"/>
-      <c r="F107" s="36"/>
-      <c r="G107" s="36"/>
-      <c r="H107" s="36"/>
-      <c r="I107" s="36"/>
-      <c r="J107" s="36"/>
-      <c r="K107" s="36"/>
-      <c r="L107" s="36"/>
-      <c r="M107" s="36"/>
-      <c r="N107" s="37"/>
-    </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C108" s="35"/>
-      <c r="D108" s="36"/>
-      <c r="E108" s="36"/>
-      <c r="F108" s="36"/>
-      <c r="G108" s="36"/>
-      <c r="H108" s="36"/>
-      <c r="I108" s="36"/>
-      <c r="J108" s="36"/>
-      <c r="K108" s="36"/>
-      <c r="L108" s="36"/>
-      <c r="M108" s="36"/>
-      <c r="N108" s="37"/>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C109" s="38"/>
-      <c r="D109" s="39"/>
-      <c r="E109" s="39"/>
-      <c r="F109" s="39"/>
-      <c r="G109" s="39"/>
-      <c r="H109" s="39"/>
-      <c r="I109" s="39"/>
-      <c r="J109" s="39"/>
-      <c r="K109" s="39"/>
-      <c r="L109" s="39"/>
-      <c r="M109" s="39"/>
-      <c r="N109" s="40"/>
-    </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C111" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
-        <v>44</v>
+      <c r="N80" s="55"/>
+      <c r="O80" s="55"/>
+      <c r="P80" s="55"/>
+      <c r="Q80" s="55"/>
+      <c r="R80" s="55"/>
+      <c r="S80" s="55"/>
+      <c r="T80" s="55"/>
+      <c r="U80" s="55"/>
+      <c r="V80" s="55"/>
+    </row>
+    <row r="81" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C81" s="29"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="30"/>
+      <c r="G81" s="30"/>
+      <c r="H81" s="30"/>
+      <c r="I81" s="30"/>
+      <c r="J81" s="30"/>
+      <c r="K81" s="31"/>
+      <c r="N81" s="55"/>
+      <c r="O81" s="55"/>
+      <c r="P81" s="55"/>
+      <c r="Q81" s="55"/>
+      <c r="R81" s="55"/>
+      <c r="S81" s="55"/>
+      <c r="T81" s="55"/>
+      <c r="U81" s="55"/>
+      <c r="V81" s="55"/>
+    </row>
+    <row r="84" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D85" s="33"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="33"/>
+      <c r="H85" s="33"/>
+      <c r="I85" s="33"/>
+      <c r="J85" s="33"/>
+      <c r="K85" s="33"/>
+      <c r="L85" s="33"/>
+      <c r="M85" s="33"/>
+      <c r="N85" s="34"/>
+    </row>
+    <row r="86" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C86" s="35"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="36"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="36"/>
+      <c r="I86" s="36"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="36"/>
+      <c r="L86" s="36"/>
+      <c r="M86" s="36"/>
+      <c r="N86" s="37"/>
+    </row>
+    <row r="87" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C87" s="35"/>
+      <c r="D87" s="36"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="36"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="36"/>
+      <c r="I87" s="36"/>
+      <c r="J87" s="36"/>
+      <c r="K87" s="36"/>
+      <c r="L87" s="36"/>
+      <c r="M87" s="36"/>
+      <c r="N87" s="37"/>
+    </row>
+    <row r="88" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C88" s="35"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="36"/>
+      <c r="F88" s="36"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="36"/>
+      <c r="I88" s="36"/>
+      <c r="J88" s="36"/>
+      <c r="K88" s="36"/>
+      <c r="L88" s="36"/>
+      <c r="M88" s="36"/>
+      <c r="N88" s="37"/>
+    </row>
+    <row r="89" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C89" s="35"/>
+      <c r="D89" s="36"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="36"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="36"/>
+      <c r="I89" s="36"/>
+      <c r="J89" s="36"/>
+      <c r="K89" s="36"/>
+      <c r="L89" s="36"/>
+      <c r="M89" s="36"/>
+      <c r="N89" s="37"/>
+    </row>
+    <row r="90" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C90" s="35"/>
+      <c r="D90" s="36"/>
+      <c r="E90" s="36"/>
+      <c r="F90" s="36"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="36"/>
+      <c r="I90" s="36"/>
+      <c r="J90" s="36"/>
+      <c r="K90" s="36"/>
+      <c r="L90" s="36"/>
+      <c r="M90" s="36"/>
+      <c r="N90" s="37"/>
+    </row>
+    <row r="91" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C91" s="35"/>
+      <c r="D91" s="36"/>
+      <c r="E91" s="36"/>
+      <c r="F91" s="36"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="36"/>
+      <c r="I91" s="36"/>
+      <c r="J91" s="36"/>
+      <c r="K91" s="36"/>
+      <c r="L91" s="36"/>
+      <c r="M91" s="36"/>
+      <c r="N91" s="37"/>
+    </row>
+    <row r="92" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C92" s="35"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="36"/>
+      <c r="F92" s="36"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="36"/>
+      <c r="I92" s="36"/>
+      <c r="J92" s="36"/>
+      <c r="K92" s="36"/>
+      <c r="L92" s="36"/>
+      <c r="M92" s="36"/>
+      <c r="N92" s="37"/>
+    </row>
+    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C93" s="35"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="36"/>
+      <c r="F93" s="36"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="36"/>
+      <c r="J93" s="36"/>
+      <c r="K93" s="36"/>
+      <c r="L93" s="36"/>
+      <c r="M93" s="36"/>
+      <c r="N93" s="37"/>
+    </row>
+    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C94" s="35"/>
+      <c r="D94" s="36"/>
+      <c r="E94" s="36"/>
+      <c r="F94" s="36"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="36"/>
+      <c r="I94" s="36"/>
+      <c r="J94" s="36"/>
+      <c r="K94" s="36"/>
+      <c r="L94" s="36"/>
+      <c r="M94" s="36"/>
+      <c r="N94" s="37"/>
+    </row>
+    <row r="95" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C95" s="38"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="39"/>
+      <c r="F95" s="39"/>
+      <c r="G95" s="39"/>
+      <c r="H95" s="39"/>
+      <c r="I95" s="39"/>
+      <c r="J95" s="39"/>
+      <c r="K95" s="39"/>
+      <c r="L95" s="39"/>
+      <c r="M95" s="39"/>
+      <c r="N95" s="40"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C41:K68"/>
-    <mergeCell ref="C72:K95"/>
+    <mergeCell ref="C34:K52"/>
+    <mergeCell ref="C56:K81"/>
     <mergeCell ref="C17:K21"/>
-    <mergeCell ref="C99:N109"/>
-    <mergeCell ref="Q17:X22"/>
-    <mergeCell ref="Q25:X35"/>
+    <mergeCell ref="C85:N95"/>
+    <mergeCell ref="Q24:X28"/>
+    <mergeCell ref="Q17:X20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3610,10 +3975,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B3:K62"/>
+  <dimension ref="B3:K70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3624,22 +3989,22 @@
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -3664,27 +4029,27 @@
     <row r="9" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C16" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
@@ -3697,7 +4062,7 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C17" s="10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -3710,7 +4075,7 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C18" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -3723,126 +4088,126 @@
     </row>
     <row r="21" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="16"/>
+        <v>66</v>
+      </c>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="19"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="49"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="19"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="49"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="19"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="49"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="19"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="49"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="19"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="49"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="17"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="19"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="49"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="20"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="22"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="52"/>
     </row>
     <row r="33" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
+      <c r="C35" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="44"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C36" s="8"/>
@@ -3868,43 +4233,149 @@
     </row>
     <row r="38" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
+      <c r="C40" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="44"/>
     </row>
     <row r="43" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="9"/>
+      <c r="B43" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C63" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="16"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C64" s="17"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="19"/>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C65" s="17"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="19"/>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C66" s="17"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="19"/>
+    </row>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C67" s="17"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="19"/>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C68" s="17"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="19"/>
+    </row>
+    <row r="69" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C69" s="17"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="19"/>
+    </row>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C70" s="20"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C63:K70"/>
+    <mergeCell ref="C40:K40"/>
+    <mergeCell ref="C35:K35"/>
+    <mergeCell ref="C23:K30"/>
     <mergeCell ref="C7:K7"/>
     <mergeCell ref="C16:K16"/>
-    <mergeCell ref="C23:K30"/>
-    <mergeCell ref="C35:K35"/>
-    <mergeCell ref="C40:K40"/>
     <mergeCell ref="C18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified for beforeEach, afterEach, beforeAll, and afterAll
</commit_message>
<xml_diff>
--- a/karma-ts-howto.xlsx
+++ b/karma-ts-howto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Ivy\Github\karma-typescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B989D3-67B1-4DE1-BD24-87FCA0A224E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFA2556-0862-46FA-80DB-AB2DC46338E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="771" firstSheet="1" activeTab="4" xr2:uid="{F8FD7D67-54D6-4F97-86DC-2E3CAB04B120}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="771" activeTab="4" xr2:uid="{F8FD7D67-54D6-4F97-86DC-2E3CAB04B120}"/>
   </bookViews>
   <sheets>
     <sheet name="Installation and Configuration" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="Sample Karma Test" sheetId="5" r:id="rId3"/>
     <sheet name="Jasmine Built-In Matchers" sheetId="8" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="10" r:id="rId5"/>
-    <sheet name="Others" sheetId="9" r:id="rId6"/>
-    <sheet name="Errors" sheetId="7" r:id="rId7"/>
+    <sheet name="Errors" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="150">
   <si>
     <t>Prerequisite:</t>
   </si>
@@ -984,18 +983,6 @@
     <t>afterEach</t>
   </si>
   <si>
-    <t>beforeAll is call once, before all the specs in describe function are run.</t>
-  </si>
-  <si>
-    <t>afterAll is called once, after all the specs  in describe function are run.</t>
-  </si>
-  <si>
-    <t>beforeEach is called before each test specification in it function is run.</t>
-  </si>
-  <si>
-    <t>afterEach is called after each test specification in it function is run.</t>
-  </si>
-  <si>
     <t>10. SyntaxError: Cannot use import statement outside a module</t>
   </si>
   <si>
@@ -1085,6 +1072,9 @@
     <t>scr/enums.ts
 scr/enums2.ts
 test/enums.ts</t>
+  </si>
+  <si>
+    <t>test/getter-setter.ts</t>
   </si>
 </sst>
 </file>
@@ -1504,18 +1494,48 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1538,36 +1558,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4615,7 +4605,7 @@
   <dimension ref="B3:O20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:O5"/>
+      <selection activeCell="H9" sqref="H9:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4625,340 +4615,342 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="57"/>
+    </row>
+    <row r="4" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="50"/>
+    </row>
+    <row r="5" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="50"/>
+    </row>
+    <row r="6" spans="2:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="60" t="s">
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="50"/>
+    </row>
+    <row r="7" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="62"/>
-    </row>
-    <row r="4" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="69" t="s">
-        <v>150</v>
-      </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="68"/>
-    </row>
-    <row r="5" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="69" t="s">
-        <v>150</v>
-      </c>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="68"/>
-    </row>
-    <row r="6" spans="2:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="63" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="69" t="s">
-        <v>152</v>
-      </c>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="68"/>
-    </row>
-    <row r="7" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="63" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="69" t="s">
-        <v>151</v>
-      </c>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="68"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="63" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="68"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="50"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="68"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="50"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="68"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="50"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="68"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="50"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="68"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="50"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="68"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="50"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="67"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="68"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="50"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="68"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="50"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="63"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="68"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="50"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="67"/>
-      <c r="O17" s="68"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="50"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="68"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="50"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="63"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="67"/>
-      <c r="O19" s="68"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="50"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="67"/>
-      <c r="L20" s="67"/>
-      <c r="M20" s="67"/>
-      <c r="N20" s="67"/>
-      <c r="O20" s="68"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="H20:O20"/>
-    <mergeCell ref="H14:O14"/>
-    <mergeCell ref="H15:O15"/>
-    <mergeCell ref="H16:O16"/>
-    <mergeCell ref="H17:O17"/>
-    <mergeCell ref="H18:O18"/>
-    <mergeCell ref="H19:O19"/>
-    <mergeCell ref="H8:O8"/>
-    <mergeCell ref="H9:O9"/>
-    <mergeCell ref="H10:O10"/>
-    <mergeCell ref="H11:O11"/>
-    <mergeCell ref="H12:O12"/>
-    <mergeCell ref="H13:O13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="H6:O6"/>
+    <mergeCell ref="H7:O7"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B9:G9"/>
@@ -4967,82 +4959,29 @@
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="H5:O5"/>
-    <mergeCell ref="H6:O6"/>
-    <mergeCell ref="H7:O7"/>
+    <mergeCell ref="H13:O13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H8:O8"/>
+    <mergeCell ref="H9:O9"/>
+    <mergeCell ref="H10:O10"/>
+    <mergeCell ref="H11:O11"/>
+    <mergeCell ref="H12:O12"/>
+    <mergeCell ref="H20:O20"/>
+    <mergeCell ref="H14:O14"/>
+    <mergeCell ref="H15:O15"/>
+    <mergeCell ref="H16:O16"/>
+    <mergeCell ref="H17:O17"/>
+    <mergeCell ref="H18:O18"/>
+    <mergeCell ref="H19:O19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6973580-6B44-46A8-AB79-589FCD55DC1A}">
-  <dimension ref="B3:B13"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="4" width="3.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA760E5-4801-49BB-909C-AFBE39FCD389}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -5172,91 +5111,91 @@
       <c r="C23" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="53"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="56"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="56"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="66"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="66"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="54"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="56"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="66"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="56"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="66"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="54"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="56"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="66"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="59"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="69"/>
     </row>
     <row r="33" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
@@ -5269,17 +5208,17 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="51"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="59"/>
+      <c r="K35" s="60"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C36" s="8"/>
@@ -5314,17 +5253,17 @@
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="50"/>
-      <c r="K40" s="51"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="60"/>
     </row>
     <row r="43" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
@@ -5347,7 +5286,7 @@
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C63" s="48" t="s">
+      <c r="C63" s="61" t="s">
         <v>95</v>
       </c>
       <c r="D63" s="22"/>
@@ -5458,47 +5397,47 @@
     </row>
     <row r="81" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C86" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="D86" s="50"/>
-      <c r="E86" s="50"/>
-      <c r="F86" s="50"/>
-      <c r="G86" s="50"/>
-      <c r="H86" s="50"/>
-      <c r="I86" s="50"/>
-      <c r="J86" s="50"/>
-      <c r="K86" s="51"/>
+      <c r="C86" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="D86" s="59"/>
+      <c r="E86" s="59"/>
+      <c r="F86" s="59"/>
+      <c r="G86" s="59"/>
+      <c r="H86" s="59"/>
+      <c r="I86" s="59"/>
+      <c r="J86" s="59"/>
+      <c r="K86" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="C16:K16"/>
+    <mergeCell ref="C18:K18"/>
     <mergeCell ref="C86:K86"/>
     <mergeCell ref="C63:K70"/>
     <mergeCell ref="C40:K40"/>
     <mergeCell ref="C35:K35"/>
     <mergeCell ref="C23:K30"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="C16:K16"/>
-    <mergeCell ref="C18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>